<commit_message>
Minor changes: - Rearranged files into another folder
</commit_message>
<xml_diff>
--- a/tof_exp_multi_perp.xlsx
+++ b/tof_exp_multi_perp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tof\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC52E3E9-1C80-460D-BFBA-84E4ADDD46A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9643099B-D50C-4AAA-A56A-6DA904A5F71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,13 +93,13 @@
     <t>disco</t>
   </si>
   <si>
-    <t>fita_3M</t>
-  </si>
-  <si>
     <t>mercosul</t>
   </si>
   <si>
     <t>reflet</t>
+  </si>
+  <si>
+    <t>fita-3M</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,7 +510,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -550,7 +550,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -570,7 +570,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -591,7 +591,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -631,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -651,7 +651,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -671,7 +671,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -711,7 +711,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -731,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -751,7 +751,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -791,7 +791,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -811,7 +811,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -831,7 +831,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -871,7 +871,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -891,7 +891,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -911,7 +911,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
@@ -951,7 +951,7 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -971,7 +971,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>

</xml_diff>